<commit_message>
updated and testing fuzzy
</commit_message>
<xml_diff>
--- a/App/bases_download_novos nomes_220527.xlsx
+++ b/App/bases_download_novos nomes_220527.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e131efba7b001de3/Pessoal/RSL Consultoria/Horizon/05-Tese Psiquiatria/tese-psiquiatria/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e131efba7b001de3/Pessoal/RSL Consultoria/Horizon/05-Tese Psiquiatria/HZN-tese-psiquiatria/App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="259" documentId="13_ncr:1_{6E4D9A89-9BBC-634A-A36E-87D371701F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{175545E7-A9F0-492C-A2E6-F49967F35D72}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="13_ncr:1_{6E4D9A89-9BBC-634A-A36E-87D371701F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8618C6F4-4D02-4E9C-9410-127528BC213E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Detalhes_da_Base" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Detalhes_da_Base!$A$1:$K$469</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Detalhes_da_Base!$A$1:$K$468</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="697">
   <si>
     <t>coluna</t>
   </si>
@@ -2074,18 +2074,12 @@
     <t>percentual_sus</t>
   </si>
   <si>
-    <t>? Qual a diferença do '% Leitos SUS / Totais'?</t>
-  </si>
-  <si>
     <t>Ação Necessária</t>
   </si>
   <si>
     <t>percentual_sm</t>
   </si>
   <si>
-    <t>? Qual a diferença do '% Profissionais SM'?</t>
-  </si>
-  <si>
     <t>etapa_filtrado</t>
   </si>
   <si>
@@ -2110,19 +2104,31 @@
     <t>Etapa filtrado</t>
   </si>
   <si>
-    <t>Tirar pois é coluna e tentar colocar em sheet separado</t>
-  </si>
-  <si>
-    <t>usar faturaremnto_presumido p/ calcular</t>
-  </si>
-  <si>
-    <t>usar numero de processos</t>
-  </si>
-  <si>
     <t>falar com rodrigo e buscar na base da transunion</t>
   </si>
   <si>
-    <t>Falar com filipe coutinho e buscar na base</t>
+    <t>gmapsCompanyName</t>
+  </si>
+  <si>
+    <t>gmapsTelephone</t>
+  </si>
+  <si>
+    <t>gmapsAddress</t>
+  </si>
+  <si>
+    <t>Usado numero de processos</t>
+  </si>
+  <si>
+    <t>Usado faturamento presumido</t>
+  </si>
+  <si>
+    <t>Usado URL Site</t>
+  </si>
+  <si>
+    <t>Usado CNPJ</t>
+  </si>
+  <si>
+    <t>Fuzzy_nome_CNESvsGMN</t>
   </si>
 </sst>
 </file>
@@ -2153,7 +2159,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2176,12 +2182,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -2215,8 +2215,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2600,11 +2600,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N474"/>
+  <dimension ref="A1:N473"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G303" sqref="G303"/>
+      <pane ySplit="1" topLeftCell="A442" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A458" sqref="A458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,7 +2639,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>676</v>
@@ -9772,7 +9772,7 @@
         <v>154</v>
       </c>
       <c r="G274" s="11" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="I274" s="5">
         <v>1</v>
@@ -9797,7 +9797,7 @@
         <v>353</v>
       </c>
       <c r="G275" s="11" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="I275" s="5">
         <v>1</v>
@@ -10042,51 +10042,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="11" t="s">
-        <v>680</v>
-      </c>
-      <c r="B285" s="11" t="s">
-        <v>680</v>
-      </c>
-      <c r="C285" s="12"/>
-      <c r="E285" s="11"/>
-      <c r="F285" s="11"/>
-      <c r="G285" s="11" t="s">
-        <v>681</v>
-      </c>
-      <c r="I285" s="11"/>
-      <c r="J285" s="11"/>
-      <c r="K285" s="11"/>
-    </row>
-    <row r="286" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="11" t="s">
+    <row r="285" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="13" t="s">
+        <v>679</v>
+      </c>
+      <c r="B285" s="13" t="s">
+        <v>679</v>
+      </c>
+      <c r="C285" s="7"/>
+      <c r="E285" s="13"/>
+      <c r="F285" s="13"/>
+      <c r="G285" s="13"/>
+      <c r="H285" s="10">
+        <v>1</v>
+      </c>
+      <c r="I285" s="13">
+        <v>0</v>
+      </c>
+      <c r="J285" s="13">
+        <v>0</v>
+      </c>
+      <c r="K285" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="13" t="s">
         <v>677</v>
       </c>
-      <c r="B286" s="11" t="s">
+      <c r="B286" s="13" t="s">
         <v>677</v>
       </c>
-      <c r="C286" s="12"/>
-      <c r="E286" s="11"/>
-      <c r="F286" s="11"/>
-      <c r="G286" s="11" t="s">
-        <v>678</v>
-      </c>
-      <c r="I286" s="11"/>
-      <c r="J286" s="11"/>
-      <c r="K286" s="11"/>
+      <c r="C286" s="7"/>
+      <c r="E286" s="13"/>
+      <c r="F286" s="13"/>
+      <c r="G286" s="13"/>
+      <c r="H286" s="10">
+        <v>1</v>
+      </c>
+      <c r="I286" s="13">
+        <v>0</v>
+      </c>
+      <c r="J286" s="13">
+        <v>0</v>
+      </c>
+      <c r="K286" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="287" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A287" s="6" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B287" s="6" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C287" s="7"/>
       <c r="E287" s="6"/>
       <c r="F287" s="6"/>
       <c r="G287" s="6"/>
+      <c r="H287" s="10">
+        <v>1</v>
+      </c>
       <c r="I287" s="6">
         <v>1</v>
       </c>
@@ -10099,15 +10116,18 @@
     </row>
     <row r="288" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" s="6" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B288" s="6" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C288" s="7"/>
       <c r="E288" s="6"/>
       <c r="F288" s="6"/>
       <c r="G288" s="6"/>
+      <c r="H288" s="10">
+        <v>1</v>
+      </c>
       <c r="I288" s="6">
         <v>1</v>
       </c>
@@ -10486,11 +10506,9 @@
       <c r="F302" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="G302" s="11" t="s">
-        <v>694</v>
-      </c>
+      <c r="G302" s="6"/>
       <c r="I302" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J302">
         <v>0</v>
@@ -10501,7 +10519,7 @@
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>59</v>
+        <v>689</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>383</v>
@@ -10513,8 +10531,9 @@
       <c r="F303" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="G303" s="11" t="s">
-        <v>694</v>
+      <c r="G303" s="6"/>
+      <c r="H303" s="1">
+        <v>1</v>
       </c>
       <c r="I303" s="5">
         <v>1</v>
@@ -10528,7 +10547,7 @@
     </row>
     <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>59</v>
+        <v>691</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>385</v>
@@ -10540,8 +10559,9 @@
       <c r="F304" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="G304" s="11" t="s">
-        <v>694</v>
+      <c r="G304" s="6"/>
+      <c r="H304" s="1">
+        <v>1</v>
       </c>
       <c r="I304" s="5">
         <v>1</v>
@@ -10555,7 +10575,7 @@
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>59</v>
+        <v>690</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>387</v>
@@ -10567,8 +10587,9 @@
       <c r="F305" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="G305" s="11" t="s">
-        <v>694</v>
+      <c r="G305" s="6"/>
+      <c r="H305" s="1">
+        <v>1</v>
       </c>
       <c r="I305" s="5">
         <v>1</v>
@@ -13721,17 +13742,11 @@
         <v>656</v>
       </c>
       <c r="G445" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="I445" s="10">
-        <v>1</v>
-      </c>
-      <c r="J445" s="10">
-        <v>1</v>
-      </c>
-      <c r="K445" s="10">
-        <v>1</v>
-      </c>
+        <v>695</v>
+      </c>
+      <c r="I445" s="10"/>
+      <c r="J445" s="10"/>
+      <c r="K445" s="10"/>
       <c r="L445" s="10"/>
       <c r="M445" s="10"/>
       <c r="N445" s="10"/>
@@ -13749,7 +13764,7 @@
         <v>19</v>
       </c>
       <c r="G446" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="I446" s="10">
         <v>1</v>
@@ -13802,7 +13817,7 @@
         <v>657</v>
       </c>
       <c r="G448" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="I448" s="10">
         <v>1</v>
@@ -13933,7 +13948,7 @@
         <v>661</v>
       </c>
       <c r="G453" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="I453" s="10">
         <v>1</v>
@@ -13964,17 +13979,11 @@
         <v>656</v>
       </c>
       <c r="G454" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="I454" s="10">
-        <v>1</v>
-      </c>
-      <c r="J454" s="10">
-        <v>1</v>
-      </c>
-      <c r="K454" s="10">
-        <v>1</v>
-      </c>
+        <v>694</v>
+      </c>
+      <c r="I454" s="10"/>
+      <c r="J454" s="10"/>
+      <c r="K454" s="10"/>
       <c r="L454" s="10"/>
       <c r="M454" s="10"/>
       <c r="N454" s="10"/>
@@ -13989,10 +13998,10 @@
         <v>663</v>
       </c>
       <c r="F455" s="10" t="s">
-        <v>12</v>
+        <v>658</v>
       </c>
       <c r="G455" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="I455" s="10">
         <v>1</v>
@@ -14017,10 +14026,10 @@
         <v>663</v>
       </c>
       <c r="F456" s="10" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="G456" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="I456" s="10">
         <v>1</v>
@@ -14045,10 +14054,10 @@
         <v>663</v>
       </c>
       <c r="F457" s="10" t="s">
-        <v>659</v>
+        <v>46</v>
       </c>
       <c r="G457" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="I457" s="10">
         <v>1</v>
@@ -14073,16 +14082,13 @@
         <v>663</v>
       </c>
       <c r="F458" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G458" s="1" t="s">
-        <v>684</v>
+        <v>50</v>
       </c>
       <c r="I458" s="10">
         <v>1</v>
       </c>
       <c r="J458" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K458" s="10">
         <v>0</v>
@@ -14101,13 +14107,16 @@
         <v>663</v>
       </c>
       <c r="F459" s="10" t="s">
-        <v>50</v>
+        <v>664</v>
+      </c>
+      <c r="G459" s="1" t="s">
+        <v>682</v>
       </c>
       <c r="I459" s="10">
         <v>1</v>
       </c>
       <c r="J459" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K459" s="10">
         <v>0</v>
@@ -14118,7 +14127,10 @@
     </row>
     <row r="460" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
-        <v>59</v>
+        <v>665</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>696</v>
       </c>
       <c r="C460" s="4"/>
       <c r="D460" s="10"/>
@@ -14126,10 +14138,11 @@
         <v>663</v>
       </c>
       <c r="F460" s="10" t="s">
-        <v>664</v>
-      </c>
-      <c r="G460" s="1" t="s">
-        <v>684</v>
+        <v>661</v>
+      </c>
+      <c r="G460" s="10"/>
+      <c r="H460" s="1">
+        <v>1</v>
       </c>
       <c r="I460" s="10">
         <v>1</v>
@@ -14146,42 +14159,35 @@
     </row>
     <row r="461" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A461" s="1" t="s">
-        <v>665</v>
+        <v>59</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C461" s="4"/>
       <c r="D461" s="10"/>
       <c r="E461" s="10" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
       <c r="F461" s="10" t="s">
-        <v>661</v>
-      </c>
-      <c r="G461" s="10"/>
-      <c r="H461" s="1">
-        <v>1</v>
-      </c>
-      <c r="I461" s="10">
-        <v>1</v>
-      </c>
-      <c r="J461" s="10">
-        <v>1</v>
-      </c>
-      <c r="K461" s="10">
-        <v>0</v>
-      </c>
+        <v>656</v>
+      </c>
+      <c r="G461" s="12" t="s">
+        <v>692</v>
+      </c>
+      <c r="I461" s="10"/>
+      <c r="J461" s="10"/>
+      <c r="K461" s="10"/>
       <c r="L461" s="10"/>
       <c r="M461" s="10"/>
       <c r="N461" s="10"/>
     </row>
     <row r="462" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
-        <v>59</v>
+        <v>668</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="C462" s="4"/>
       <c r="D462" s="10"/>
@@ -14189,10 +14195,11 @@
         <v>667</v>
       </c>
       <c r="F462" s="10" t="s">
-        <v>656</v>
-      </c>
-      <c r="G462" s="13" t="s">
-        <v>692</v>
+        <v>657</v>
+      </c>
+      <c r="G462" s="10"/>
+      <c r="H462" s="1">
+        <v>1</v>
       </c>
       <c r="I462" s="10">
         <v>1</v>
@@ -14201,7 +14208,7 @@
         <v>1</v>
       </c>
       <c r="K462" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L462" s="10"/>
       <c r="M462" s="10"/>
@@ -14209,32 +14216,25 @@
     </row>
     <row r="463" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A463" s="1" t="s">
-        <v>668</v>
+        <v>59</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="C463" s="4"/>
       <c r="D463" s="10"/>
       <c r="E463" s="10" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="F463" s="10" t="s">
-        <v>657</v>
-      </c>
-      <c r="G463" s="10"/>
-      <c r="H463" s="1">
-        <v>1</v>
-      </c>
-      <c r="I463" s="10">
-        <v>1</v>
-      </c>
-      <c r="J463" s="10">
-        <v>1</v>
-      </c>
-      <c r="K463" s="10">
-        <v>0</v>
-      </c>
+        <v>656</v>
+      </c>
+      <c r="G463" s="12" t="s">
+        <v>693</v>
+      </c>
+      <c r="I463" s="10"/>
+      <c r="J463" s="10"/>
+      <c r="K463" s="10"/>
       <c r="L463" s="10"/>
       <c r="M463" s="10"/>
       <c r="N463" s="10"/>
@@ -14242,9 +14242,6 @@
     <row r="464" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B464" s="1" t="s">
-        <v>670</v>
       </c>
       <c r="C464" s="4"/>
       <c r="D464" s="10"/>
@@ -14252,10 +14249,10 @@
         <v>669</v>
       </c>
       <c r="F464" s="10" t="s">
-        <v>656</v>
-      </c>
-      <c r="G464" s="13" t="s">
-        <v>691</v>
+        <v>19</v>
+      </c>
+      <c r="G464" s="1" t="s">
+        <v>684</v>
       </c>
       <c r="I464" s="10">
         <v>1</v>
@@ -14264,7 +14261,7 @@
         <v>1</v>
       </c>
       <c r="K464" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L464" s="10"/>
       <c r="M464" s="10"/>
@@ -14280,10 +14277,10 @@
         <v>669</v>
       </c>
       <c r="F465" s="10" t="s">
-        <v>19</v>
+        <v>657</v>
       </c>
       <c r="G465" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="I465" s="10">
         <v>1</v>
@@ -14299,8 +14296,8 @@
       <c r="N465" s="10"/>
     </row>
     <row r="466" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A466" s="1" t="s">
-        <v>59</v>
+      <c r="B466" s="1" t="s">
+        <v>671</v>
       </c>
       <c r="C466" s="4"/>
       <c r="D466" s="10"/>
@@ -14308,10 +14305,10 @@
         <v>669</v>
       </c>
       <c r="F466" s="10" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="G466" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I466" s="10">
         <v>1</v>
@@ -14327,36 +14324,28 @@
       <c r="N466" s="10"/>
     </row>
     <row r="467" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B467" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="C467" s="4"/>
+      <c r="A467" s="1" t="s">
+        <v>672</v>
+      </c>
       <c r="D467" s="10"/>
       <c r="E467" s="10" t="s">
-        <v>669</v>
-      </c>
-      <c r="F467" s="10" t="s">
-        <v>661</v>
-      </c>
-      <c r="G467" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="I467" s="10">
-        <v>1</v>
-      </c>
-      <c r="J467" s="10">
-        <v>1</v>
-      </c>
-      <c r="K467" s="10">
-        <v>0</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F467" s="10"/>
+      <c r="G467" s="10"/>
+      <c r="H467" s="1">
+        <v>1</v>
+      </c>
+      <c r="I467" s="10"/>
+      <c r="J467" s="10"/>
+      <c r="K467" s="10"/>
       <c r="L467" s="10"/>
       <c r="M467" s="10"/>
       <c r="N467" s="10"/>
     </row>
     <row r="468" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A468" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D468" s="10"/>
       <c r="E468" s="10" t="s">
@@ -14375,18 +14364,10 @@
       <c r="N468" s="10"/>
     </row>
     <row r="469" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A469" s="1" t="s">
-        <v>673</v>
-      </c>
       <c r="D469" s="10"/>
-      <c r="E469" s="10" t="s">
-        <v>59</v>
-      </c>
+      <c r="E469" s="10"/>
       <c r="F469" s="10"/>
       <c r="G469" s="10"/>
-      <c r="H469" s="1">
-        <v>1</v>
-      </c>
       <c r="I469" s="10"/>
       <c r="J469" s="10"/>
       <c r="K469" s="10"/>
@@ -14442,20 +14423,8 @@
       <c r="M473" s="10"/>
       <c r="N473" s="10"/>
     </row>
-    <row r="474" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D474" s="10"/>
-      <c r="E474" s="10"/>
-      <c r="F474" s="10"/>
-      <c r="G474" s="10"/>
-      <c r="I474" s="10"/>
-      <c r="J474" s="10"/>
-      <c r="K474" s="10"/>
-      <c r="L474" s="10"/>
-      <c r="M474" s="10"/>
-      <c r="N474" s="10"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K469" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K468" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>

</xml_diff>